<commit_message>
added inpatient total cost variables
</commit_message>
<xml_diff>
--- a/lookup.xlsx
+++ b/lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyakesarwani/Documents/GitHub/hospital-cost-reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96143A15-BEFF-3E40-920C-A7BA61242EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CA38C9-2FCD-7448-B8F1-736C2F99E18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="760" windowWidth="22900" windowHeight="18880" activeTab="1" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
+    <workbookView xWindow="160" yWindow="760" windowWidth="13360" windowHeight="18880" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Table" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="207">
   <si>
     <t>rec</t>
   </si>
@@ -590,17 +590,90 @@
     <t>inpatient total costs</t>
   </si>
   <si>
-    <t>20000</t>
+    <t>i_adultandpeds_cost</t>
+  </si>
+  <si>
+    <t>i_icu_cost</t>
+  </si>
+  <si>
+    <t>i_ccu_cost</t>
+  </si>
+  <si>
+    <t>i_bicu_cost</t>
+  </si>
+  <si>
+    <t>i_sicu_cost</t>
+  </si>
+  <si>
+    <t>i_otherspecial_cost</t>
+  </si>
+  <si>
+    <t>i_subprovideripf_cost</t>
+  </si>
+  <si>
+    <t>i_subproviderirf_cost</t>
+  </si>
+  <si>
+    <t>i_subprovider_cost</t>
+  </si>
+  <si>
+    <t>i_nursery_cost</t>
+  </si>
+  <si>
+    <t>i_skillednursing_cost</t>
+  </si>
+  <si>
+    <t>i_nursing_cost</t>
+  </si>
+  <si>
+    <t>i_otherlongterm_cost</t>
+  </si>
+  <si>
+    <t>03200</t>
+  </si>
+  <si>
+    <t>03300</t>
+  </si>
+  <si>
+    <t>03400</t>
+  </si>
+  <si>
+    <t>03500</t>
+  </si>
+  <si>
+    <t>04000</t>
+  </si>
+  <si>
+    <t>04100</t>
+  </si>
+  <si>
+    <t>04400</t>
+  </si>
+  <si>
+    <t>04301</t>
+  </si>
+  <si>
+    <t>04500</t>
+  </si>
+  <si>
+    <t>04600</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -626,9 +699,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -943,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC2BB4DF-E65D-224C-B8BB-1875153B4956}">
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScale="108" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92:G92"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="119" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2833,16 +2907,16 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B92" t="s">
         <v>182</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>184</v>
+        <v>44</v>
       </c>
       <c r="E92"/>
       <c r="F92">
@@ -2852,8 +2926,245 @@
         <v>1</v>
       </c>
     </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B93" t="s">
+        <v>182</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F93">
+        <v>10</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+    </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D94"/>
+      <c r="A94" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B94" t="s">
+        <v>182</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F94">
+        <v>10</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B95" t="s">
+        <v>182</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F95">
+        <v>10</v>
+      </c>
+      <c r="G95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B96" t="s">
+        <v>182</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F96">
+        <v>10</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B97" t="s">
+        <v>182</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F97">
+        <v>10</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B98" t="s">
+        <v>182</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F98">
+        <v>10</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B99" t="s">
+        <v>182</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F99">
+        <v>10</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B100" t="s">
+        <v>182</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F100">
+        <v>10</v>
+      </c>
+      <c r="G100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B101" t="s">
+        <v>182</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F101">
+        <v>10</v>
+      </c>
+      <c r="G101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B102" t="s">
+        <v>182</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F102">
+        <v>10</v>
+      </c>
+      <c r="G102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B103" t="s">
+        <v>182</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F103">
+        <v>10</v>
+      </c>
+      <c r="G103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B104" t="s">
+        <v>182</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F104">
+        <v>10</v>
+      </c>
+      <c r="G104">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2865,8 +3176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F01AFD1-3AE8-2C43-8863-F91A96C0A348}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
changed flow to dollar_flow
</commit_message>
<xml_diff>
--- a/lookup.xlsx
+++ b/lookup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyakesarwani/Documents/GitHub/hospital-cost-reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C44352B-8092-BD4D-86F0-93B9D8DFFAD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA71952-05C9-1643-A80A-C4EF04D21795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="760" windowWidth="13360" windowHeight="18880" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
   </bookViews>
@@ -1053,7 +1053,7 @@
   <dimension ref="A1:G104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" zoomScale="89" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3210,7 +3210,7 @@
   <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3752,8 +3752,8 @@
       <c r="A49" t="s">
         <v>182</v>
       </c>
-      <c r="B49" t="s">
-        <v>108</v>
+      <c r="B49" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C49" t="s">
         <v>205</v>
@@ -3763,8 +3763,8 @@
       <c r="A50" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B50" t="s">
-        <v>108</v>
+      <c r="B50" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C50" t="s">
         <v>206</v>
@@ -3774,8 +3774,8 @@
       <c r="A51" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B51" t="s">
-        <v>108</v>
+      <c r="B51" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C51" t="s">
         <v>207</v>
@@ -3785,8 +3785,8 @@
       <c r="A52" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B52" t="s">
-        <v>108</v>
+      <c r="B52" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C52" t="s">
         <v>208</v>
@@ -3796,8 +3796,8 @@
       <c r="A53" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B53" t="s">
-        <v>108</v>
+      <c r="B53" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C53" t="s">
         <v>209</v>
@@ -3807,8 +3807,8 @@
       <c r="A54" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B54" t="s">
-        <v>108</v>
+      <c r="B54" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C54" t="s">
         <v>210</v>
@@ -3818,8 +3818,8 @@
       <c r="A55" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B55" t="s">
-        <v>108</v>
+      <c r="B55" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C55" t="s">
         <v>211</v>
@@ -3829,8 +3829,8 @@
       <c r="A56" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B56" t="s">
-        <v>108</v>
+      <c r="B56" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C56" t="s">
         <v>212</v>
@@ -3840,8 +3840,8 @@
       <c r="A57" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B57" t="s">
-        <v>108</v>
+      <c r="B57" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C57" t="s">
         <v>213</v>
@@ -3851,8 +3851,8 @@
       <c r="A58" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B58" t="s">
-        <v>108</v>
+      <c r="B58" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C58" t="s">
         <v>214</v>
@@ -3862,8 +3862,8 @@
       <c r="A59" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B59" t="s">
-        <v>108</v>
+      <c r="B59" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C59" t="s">
         <v>215</v>
@@ -3873,8 +3873,8 @@
       <c r="A60" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B60" t="s">
-        <v>108</v>
+      <c r="B60" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C60" t="s">
         <v>216</v>
@@ -3884,8 +3884,8 @@
       <c r="A61" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B61" t="s">
-        <v>108</v>
+      <c r="B61" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C61" t="s">
         <v>217</v>

</xml_diff>

<commit_message>
added costs to lookup
</commit_message>
<xml_diff>
--- a/lookup.xlsx
+++ b/lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyakesarwani/Documents/GitHub/hospital-cost-reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D069E228-3145-E14B-B12A-2E62E06ABACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D8E7F0-2119-804D-A573-6929BECE8E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="760" windowWidth="13360" windowHeight="18880" activeTab="1" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
+    <workbookView xWindow="160" yWindow="760" windowWidth="13360" windowHeight="18880" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Table" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="222">
   <si>
     <t>rec</t>
   </si>
@@ -696,6 +696,12 @@
   </si>
   <si>
     <t>Medicaid total cost</t>
+  </si>
+  <si>
+    <t>chip_totcost</t>
+  </si>
+  <si>
+    <t>CHIP total cost</t>
   </si>
 </sst>
 </file>
@@ -1063,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC2BB4DF-E65D-224C-B8BB-1875153B4956}">
-  <dimension ref="A1:G105"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" zoomScale="89" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="89" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3232,6 +3238,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F106">
+        <v>10</v>
+      </c>
+      <c r="G106">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3240,10 +3266,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F01AFD1-3AE8-2C43-8863-F91A96C0A348}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3935,6 +3961,17 @@
         <v>219</v>
       </c>
     </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C63" t="s">
+        <v>221</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>